<commit_message>
new account mapping process updating functions, need to test all
</commit_message>
<xml_diff>
--- a/excel/example-ReverseSplitLog.xlsx
+++ b/excel/example-ReverseSplitLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaff\Documents\Python\github\auto-rsa\main\RSAssistant\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaff\Documents\Python\github\orderFlowbot\main\RSAssistant\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238BA34-CE4F-499F-B076-9B0172752DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABE2B1D-F3FD-4F70-96B4-9185C365ABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20820" yWindow="1185" windowWidth="18600" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26640" yWindow="735" windowWidth="18600" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reverse Split Log" sheetId="3" r:id="rId1"/>
@@ -298,7 +298,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -326,8 +326,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -337,7 +335,12 @@
     <cellStyle name="Default Dark" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.1498764000366222"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.1498764000366222"/>
@@ -600,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33956B6D-9B83-4260-B581-B76FA865052C}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -614,9 +617,11 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="13.125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10">
         <f>SUM(42:42)</f>
         <v>0</v>
@@ -641,8 +646,10 @@
         <f>E2</f>
         <v>45426</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -657,8 +664,10 @@
         <v>45426</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -677,304 +686,380 @@
       <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>3</v>
       </c>
@@ -997,10 +1082,21 @@
         <f>SUMIF(F4:F40,"&gt;0")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G41" s="6">
+        <f>SUM(G4:G40)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="6">
+        <f>SUMIF(H4:H40,"&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
+      <c r="B42" s="10">
+        <f>SUM(C42:K42)</f>
+        <v>0</v>
+      </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9">
         <f>D41-C41</f>
@@ -1011,11 +1107,21 @@
         <f>F41-E41</f>
         <v>0</v>
       </c>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9">
+        <f>H41-G41</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:F42">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",C4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:H42">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",C4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N/A",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1026,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1040,44 +1146,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>1234</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -1094,7 +1200,7 @@
       <c r="B5" s="13">
         <v>1</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>1234</v>
       </c>
       <c r="D5" s="13" t="s">

</xml_diff>